<commit_message>
React Render & React Hooks
</commit_message>
<xml_diff>
--- a/DSA/Problems/DSA Questions.xlsx
+++ b/DSA/Problems/DSA Questions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1844" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1850" uniqueCount="648">
   <si>
     <t>S.No</t>
   </si>
@@ -1967,10 +1967,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="37">
     <font>
@@ -2098,9 +2098,16 @@
       <scheme val="major"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2113,11 +2120,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2129,25 +2167,34 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2166,40 +2213,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2212,31 +2227,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2299,7 +2299,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2311,49 +2341,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2377,6 +2371,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2389,7 +2395,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2401,55 +2449,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2510,6 +2510,15 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -2530,11 +2539,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2554,17 +2569,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2577,162 +2588,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3177,8 +3177,8 @@
   <sheetPr/>
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="19.6" outlineLevelCol="3"/>
@@ -3710,7 +3710,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" ht="26" spans="1:3">
+    <row r="41" ht="26" spans="1:4">
       <c r="A41" s="31">
         <v>40</v>
       </c>
@@ -3720,8 +3720,11 @@
       <c r="C41" s="33" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" ht="26" spans="1:3">
+      <c r="D41" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" ht="26" spans="1:4">
       <c r="A42" s="31">
         <v>41</v>
       </c>
@@ -3731,8 +3734,11 @@
       <c r="C42" s="33" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="43" ht="26" spans="1:3">
+      <c r="D42" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" ht="26" spans="1:4">
       <c r="A43" s="31">
         <v>42</v>
       </c>
@@ -3742,8 +3748,11 @@
       <c r="C43" s="33" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="44" ht="26" spans="1:3">
+      <c r="D43" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" ht="26" spans="1:4">
       <c r="A44" s="31">
         <v>43</v>
       </c>
@@ -3753,8 +3762,11 @@
       <c r="C44" s="35" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="45" ht="26" spans="1:3">
+      <c r="D44" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" ht="26" spans="1:4">
       <c r="A45" s="31">
         <v>44</v>
       </c>
@@ -3764,8 +3776,11 @@
       <c r="C45" s="34" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="46" ht="26" spans="1:3">
+      <c r="D45" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" ht="26" spans="1:4">
       <c r="A46" s="31">
         <v>45</v>
       </c>
@@ -3774,6 +3789,9 @@
       </c>
       <c r="C46" s="34" t="s">
         <v>55</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="47" ht="26" spans="1:3">

</xml_diff>